<commit_message>
Update output format: Remove original lock column and clean hex format
- Remove original 'lock' column from final output
- Rename 'lock hex' to 'lock id'
- Remove '0x' prefix from hexadecimal values (e.g., 55062  d716 instead of 0xd716)
- Update UI descriptions and documentation to reflect new behavior
- Update test files to match new expected output format
- Final columns are now: lock id, fsu, start, end
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,150 +436,130 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>lock</t>
+          <t>lock id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>lock hex</t>
+          <t>fsu</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>fsu</t>
+          <t>start</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>end</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>55062</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>d716</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0xd716</t>
+          <t>3-9-2-8</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3-9-2-8</t>
+          <t>2025-09-16 00:00:00 +0000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-09-16 00:00:00 +0000</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
         <is>
           <t>2025-09-16 04:00:00 +0000</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>55063</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>d717</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0xd717</t>
+          <t>3-9-2-9</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3-9-2-9</t>
+          <t>2025-09-16 04:00:00 +0000</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-09-16 04:00:00 +0000</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
         <is>
           <t>2025-09-16 08:00:00 +0000</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>55064</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>d718</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0xd718</t>
+          <t>3-9-2-10</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3-9-2-10</t>
+          <t>2025-09-16 08:00:00 +0000</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-09-16 08:00:00 +0000</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
         <is>
           <t>2025-09-16 12:00:00 +0000</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>55065</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>d719</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0xd719</t>
+          <t>3-9-2-11</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3-9-2-11</t>
+          <t>2025-09-16 12:00:00 +0000</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
-        <is>
-          <t>2025-09-16 12:00:00 +0000</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
         <is>
           <t>2025-09-16 16:00:00 +0000</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>55066</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>d71a</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0xd71a</t>
+          <t>3-9-2-12</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3-9-2-12</t>
+          <t>2025-09-16 16:00:00 +0000</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>2025-09-16 16:00:00 +0000</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>2025-09-16 20:00:00 +0000</t>
         </is>

</xml_diff>